<commit_message>
2019-10-01 Commit : 1
</commit_message>
<xml_diff>
--- a/mini_project/add_items.xlsx
+++ b/mini_project/add_items.xlsx
@@ -28,12 +28,9 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="0.531cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.267cm"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.267cm"/>
-    </style:style>
-    <style:style style:name="co3" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="3.445cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
@@ -41,21 +38,21 @@
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
+    </style:style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:border="0.002cm solid #000000"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:table table:name="Sheet1" table:style-name="ta1" table:print="false">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce1"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="ce1"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce1"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
             <text:p>shop_id</text:p>
           </table:table-cell>
@@ -67,11 +64,6 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
           <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
@@ -84,11 +76,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -100,11 +87,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -116,11 +98,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -132,11 +109,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -148,11 +120,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -164,11 +131,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -180,11 +142,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -196,11 +153,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -212,11 +164,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -228,11 +175,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -244,11 +186,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -260,11 +197,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -276,11 +208,6 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
             <text:p>rjpt0003</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
@@ -291,151 +218,52 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s text:c="2"/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="4"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>
-              <text:s/>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" office:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
         </table:table-row>
       </table:table>
     </office:spreadsheet>
@@ -447,8 +275,10 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:generator>OpenOffice/4.1.2$Win32 OpenOffice.org_project/412m3$Build-9782</meta:generator>
-    <dc:date>2019-09-25T14:12:00.96</dc:date>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="84" meta:object-count="0"/>
+    <dc:date>2019-09-30T13:30:56.16</dc:date>
+    <meta:editing-duration>PT2M44S</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="51" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -457,17 +287,17 @@
 <office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:ooo="http://openoffice.org/2004/office" office:version="1.2">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
-      <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
+      <config:config-item config:name="VisibleAreaTop" config:type="int">451</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">8477</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">15355</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">7948</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">9484</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">16</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">10</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -635,9 +465,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2019-09-25">25/09/2019</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2019-09-30">30/09/2019</text:date>
             , 
-            <text:time>14:12:00</text:time>
+            <text:time>13:30:56</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>